<commit_message>
Pianificazione del 3 Sprint
</commit_message>
<xml_diff>
--- a/docs/Sprint Planning.xlsx
+++ b/docs/Sprint Planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\PycharmProjects\Progetto-SAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DE1E23-C1FF-42A0-BE13-011E03BB924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4D3944-5E46-4083-8A5C-3E84B9A367BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1745140-38CB-4D37-89A1-E6CB77C188BD}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{D1745140-38CB-4D37-89A1-E6CB77C188BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
   <si>
     <t>User Story</t>
   </si>
@@ -96,6 +96,33 @@
   </si>
   <si>
     <t>Totale:</t>
+  </si>
+  <si>
+    <t>1.    Operazione Annulla</t>
+  </si>
+  <si>
+    <t>2.    Operazione Porta avanti</t>
+  </si>
+  <si>
+    <t>3.     Operazione Porta dietro</t>
+  </si>
+  <si>
+    <t>4.     Modifica zoom</t>
+  </si>
+  <si>
+    <t>5.    Superfice spazio di lavoro</t>
+  </si>
+  <si>
+    <t>6.    Attivazione griglia</t>
+  </si>
+  <si>
+    <t>7.    Disattivazione Griglia</t>
+  </si>
+  <si>
+    <t>8.    Dimensione griglia</t>
+  </si>
+  <si>
+    <t>Media</t>
   </si>
 </sst>
 </file>
@@ -166,7 +193,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +220,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,9 +279,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,15 +295,15 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutrale" xfId="1" builtinId="28"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
     <dxf>
       <font>
         <strike val="0"/>
@@ -352,6 +388,45 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
         <family val="1"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -418,6 +493,43 @@
         <vertAlign val="baseline"/>
         <sz val="14"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <family val="1"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -1074,24 +1186,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8C5124B2-2BFF-47E9-9623-5280698D06A7}" name="Tabella7" displayName="Tabella7" ref="I4:K11" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8C5124B2-2BFF-47E9-9623-5280698D06A7}" name="Tabella7" displayName="Tabella7" ref="I4:K11" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="I4:K11" xr:uid="{8C5124B2-2BFF-47E9-9623-5280698D06A7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9647693D-C193-40C0-B3F0-A64009CEA3EA}" name="User Story" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{49055050-66D8-485F-A478-63DE194D58C1}" name="Priority" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{1105F612-A83F-4FE5-BDA9-3B5B8406C423}" name="Story Points" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9647693D-C193-40C0-B3F0-A64009CEA3EA}" name="User Story" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{49055050-66D8-485F-A478-63DE194D58C1}" name="Priority" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{1105F612-A83F-4FE5-BDA9-3B5B8406C423}" name="Story Points" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D2DCBFBB-65B8-4EE9-9159-784CB57BDB17}" name="Tabella8" displayName="Tabella8" ref="I16:K22" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D2DCBFBB-65B8-4EE9-9159-784CB57BDB17}" name="Tabella8" displayName="Tabella8" ref="I16:K22" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="I16:K22" xr:uid="{D2DCBFBB-65B8-4EE9-9159-784CB57BDB17}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CD07ED07-E180-4BC8-A42A-11715B333976}" name="User Story" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{85B8C0DB-DF98-436D-B0E0-14F5BABDE74C}" name="Priority" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{DD517DFE-3284-4872-AFB0-5B7CB4B828BD}" name="Story Points" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{CD07ED07-E180-4BC8-A42A-11715B333976}" name="User Story" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{85B8C0DB-DF98-436D-B0E0-14F5BABDE74C}" name="Priority" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{DD517DFE-3284-4872-AFB0-5B7CB4B828BD}" name="Story Points" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64F2D72A-FFB7-48D0-99D9-541741FDC05A}" name="Tabella82" displayName="Tabella82" ref="I27:K35" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="I27:K35" xr:uid="{64F2D72A-FFB7-48D0-99D9-541741FDC05A}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{AB38B270-5F9C-4489-BFDD-91FFE1D9FD5A}" name="User Story" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{DDA9E87B-1CD3-4FA1-AA72-2B66DE008775}" name="Priority" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{6F09F731-FA49-471F-A7C8-889B3F1AF530}" name="Story Points" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1414,33 +1538,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1904DCC9-2836-4A50-8205-27238C2B9945}">
-  <dimension ref="A3:K31"/>
+  <dimension ref="A3:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="65" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.36328125" customWidth="1"/>
     <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
-      <c r="I3" s="10" t="s">
+    <row r="3" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="10"/>
+      <c r="I3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1473,7 +1597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1484,7 +1608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1495,7 +1619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1506,7 +1630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I10" s="5" t="s">
         <v>9</v>
       </c>
@@ -1517,7 +1641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1528,7 +1652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="I12" s="8"/>
@@ -1540,26 +1664,26 @@
         <v>22 story points</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I15" s="12" t="s">
+    <row r="15" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+    </row>
+    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
@@ -1570,7 +1694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I17" s="5" t="s">
         <v>11</v>
       </c>
@@ -1581,7 +1705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I18" s="5" t="s">
         <v>12</v>
       </c>
@@ -1592,7 +1716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I19" s="5" t="s">
         <v>13</v>
       </c>
@@ -1603,7 +1727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I20" s="5" t="s">
         <v>14</v>
       </c>
@@ -1614,7 +1738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D21" s="2"/>
       <c r="I21" s="5" t="s">
         <v>15</v>
@@ -1626,7 +1750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="I22" s="5" t="s">
         <v>16</v>
       </c>
@@ -1637,7 +1761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I23" s="8"/>
       <c r="J23" s="9" t="s">
         <v>19</v>
@@ -1647,73 +1771,178 @@
         <v>20 story points</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I26" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" spans="1:11" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
+      <c r="I31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="I32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K32" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="9:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="I33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="9:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="I34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="9:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="I35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="9:11" ht="20" x14ac:dyDescent="0.35">
+      <c r="J36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" s="9" t="str">
+        <f>SUM(Tabella82[Story Points]) &amp; " story points"</f>
+        <v>26 story points</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1944,20 +2173,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1980,6 +2209,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498596A7-47B0-45CF-94DF-505062FDA0AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3068FBC-AB4C-435F-AF67-0DCCBD638E93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1987,12 +2224,4 @@
     <ds:schemaRef ds:uri="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498596A7-47B0-45CF-94DF-505062FDA0AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>